<commit_message>
Removed some unusable comments; Added union re. expr. for tags cleaning; Add replacement for html entity &nbsp; Try to find prev. question links in part [who_asks]; Extend reg. exprs. for parts [previous], [who_asks], [who_answers], [answer]; Extend sql script with query: Find doubles in one row; Fix bug for func. readFileAsLinesLst; Added reading multiple files at a time;
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sources\Python\HandHelp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{076463F5-2097-4729-ADEE-DE089E6B2F5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92171151-48C2-407D-A7CC-EF160D6A9A7C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="27945" windowHeight="16440" xr2:uid="{6E115BE8-15E2-46DE-BAF8-951F24604858}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>61, 83, 187, 188, 189, 190, 191, 192</t>
   </si>
@@ -58,13 +58,31 @@
   </si>
   <si>
     <t>Диапазон до</t>
+  </si>
+  <si>
+    <t>6059, 6122, 6123, 6124, 6125, 6126, 6127, 6128, 6129, 6130, 6131, 6132, 6133, 6134, 6135, 6136, 6137, 6138, 6139, 6140, 6141, 6142, 6143, 6144, 6145, 6146, 6147, 6148, 6149, 6150, 6151, 6152, 6153, 6154, 6155, 6156, 6157, 6158, 6159, 6160, 6161, 6162, 6163, 6164, 6165, 6440, 6517, 6518, 6519, 6520, 6642, 6643, 6644, 6645, 6646, 6647, 6648, 6649, 6650, 6651, 6652, 6653, 6654, 6655, 6656, 6657, 6658, 6728</t>
+  </si>
+  <si>
+    <t>8073, 8086, 8706, 8797, 8879</t>
+  </si>
+  <si>
+    <t>10062, 10070, 10127, 10432, 10436, 10441, 10463, 10470, 10501, 10577, 10584, 10589, 10595, 10609, 10671, 10761, 10762, 10888, 10959</t>
+  </si>
+  <si>
+    <t>11099, 11306, 11307, 11358, 11384, 11427, 11428, 11709, 11990</t>
+  </si>
+  <si>
+    <t>12014, 12279, 12295, 12417, 12579</t>
+  </si>
+  <si>
+    <t>13061, 13123, 13125, 13209, 13217, 13465, 13496</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -84,6 +102,15 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -131,19 +158,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -462,7 +492,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -475,19 +505,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -495,16 +525,16 @@
       <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="5">
         <v>1000</v>
       </c>
       <c r="C2" s="1">
-        <v>994</v>
+        <v>996</v>
       </c>
       <c r="D2" s="1">
-        <v>21</v>
-      </c>
-      <c r="E2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -512,7 +542,7 @@
       <c r="A3" s="4">
         <v>1001</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="5">
         <v>2000</v>
       </c>
       <c r="C3" s="1">
@@ -521,7 +551,7 @@
       <c r="D3" s="1">
         <v>30</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="3" t="s">
         <v>1</v>
       </c>
     </row>
@@ -529,7 +559,7 @@
       <c r="A4" s="4">
         <v>2001</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="5">
         <v>3000</v>
       </c>
       <c r="C4" s="1">
@@ -538,7 +568,7 @@
       <c r="D4" s="1">
         <v>16</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="3" t="s">
         <v>2</v>
       </c>
     </row>
@@ -546,7 +576,7 @@
       <c r="A5" s="4">
         <v>3001</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="5">
         <v>4000</v>
       </c>
       <c r="C5" s="1">
@@ -555,7 +585,7 @@
       <c r="D5" s="1">
         <v>10</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="3" t="s">
         <v>2</v>
       </c>
     </row>
@@ -563,7 +593,7 @@
       <c r="A6" s="4">
         <v>4001</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="5">
         <v>5000</v>
       </c>
       <c r="C6" s="1">
@@ -572,7 +602,7 @@
       <c r="D6" s="1">
         <v>18</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="3" t="s">
         <v>2</v>
       </c>
     </row>
@@ -580,7 +610,7 @@
       <c r="A7" s="4">
         <v>5001</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="5">
         <v>6000</v>
       </c>
       <c r="C7" s="1">
@@ -589,97 +619,145 @@
       <c r="D7" s="1">
         <v>7</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>6001</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="5">
         <v>7000</v>
       </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
+      <c r="C8" s="1">
+        <v>932</v>
+      </c>
+      <c r="D8" s="1">
+        <v>14</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>7001</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="5">
         <v>8000</v>
       </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
+      <c r="C9" s="1">
+        <v>999</v>
+      </c>
+      <c r="D9" s="1">
+        <v>14</v>
+      </c>
+      <c r="E9" s="3">
+        <v>7236</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>8001</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="5">
         <v>9000</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
+      <c r="C10" s="1">
+        <v>996</v>
+      </c>
+      <c r="D10" s="1">
+        <v>3</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>9001</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="5">
         <v>10000</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C11" s="1">
+        <v>996</v>
+      </c>
+      <c r="D11" s="1">
+        <v>7</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>10001</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="5">
         <v>11000</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
+      <c r="C12" s="1">
+        <v>982</v>
+      </c>
+      <c r="D12" s="1">
+        <v>3</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>11001</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="5">
         <v>12000</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
+      <c r="C13" s="1">
+        <v>992</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>12001</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="5">
         <v>13000</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
+      <c r="C14" s="1">
+        <v>995</v>
+      </c>
+      <c r="D14" s="1">
+        <v>8</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>13001</v>
       </c>
-      <c r="B15" s="2">
-        <v>14000</v>
-      </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
+      <c r="B15" s="5">
+        <v>13520</v>
+      </c>
+      <c r="C15" s="1">
+        <v>513</v>
+      </c>
+      <c r="D15" s="1">
+        <v>3</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>